<commit_message>
fix comodity doesnt match the hint of the hard code
</commit_message>
<xml_diff>
--- a/JF25024/invoice_output/CT&INV&PL JF25024 FOB.xlsx
+++ b/JF25024/invoice_output/CT&INV&PL JF25024 FOB.xlsx
@@ -1692,7 +1692,7 @@
         <v>49418.3</v>
       </c>
       <c r="D16" s="111">
-        <f>IFERROR(E16/C16,0)</f>
+        <f>E16/C16</f>
         <v/>
       </c>
       <c r="E16" s="111" t="n">
@@ -1714,7 +1714,7 @@
         <v>152159.1</v>
       </c>
       <c r="D17" s="111">
-        <f>IFERROR(E17/C17,0)</f>
+        <f>E17/C17</f>
         <v/>
       </c>
       <c r="E17" s="111" t="n">
@@ -2416,7 +2416,7 @@
         <v>49418.3</v>
       </c>
       <c r="F22" s="123">
-        <f>IFERROR(G22/E22,0)</f>
+        <f>G22/E22</f>
         <v/>
       </c>
       <c r="G22" s="123" t="n">
@@ -2448,7 +2448,7 @@
         <v>152159.1</v>
       </c>
       <c r="F23" s="123">
-        <f>IFERROR(G23/E23,0)</f>
+        <f>G23/E23</f>
         <v/>
       </c>
       <c r="G23" s="123" t="n">

</xml_diff>